<commit_message>
atualização de código + caixa de seleção
</commit_message>
<xml_diff>
--- a/manutencoes.xlsx
+++ b/manutencoes.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,8 +441,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -452,6 +454,601 @@
       <c r="C2" t="inlineStr">
         <is>
           <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>banheiro B1 masculino - 2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>banheiro B2 masculino - Exclusivo gerência</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>banheiro B2 feminino - Exclusivo gerência</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>banheiro B3 feminino</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>banheiro B3 feminino - 2</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>banheiro B4 unissex</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>banheiro B4 feminino</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>vestiario B5 feminino -  Armários e area de descanso</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>vestiario B5 feminino - Vasos e Chuveiros</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>vestiario B6 feminino -  Armários e area de descanso</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>vestiario B6 feminino - Vasos e Chuveiros</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>vestiario B7 masculino - Armários e area de descanso</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>vestiario B7 masculino - Vasos e Chuveiros</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>banheiro B8 masculino</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>banheiro B8 feminino</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>banheiro B9 masculino - trancado</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>banheiro B9 feminino - trancado</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>banheiro B11 masculino - exclusivo</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>banheiro B11 feminino - virou DML</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>banheiro B12 UNISSEX - exclusivo</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>banheiro B12 feminino</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>banheiro B13 UNISSEX - exclusivo</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>banheiro B13 feminino</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>banheiro B14 masculino</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>banheiro B14 feminino</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>banheiro B15 masculino</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>banheiro B15 feminino</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>vestiario B16 masculino - Vasos e Chuveiros</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>vestiario B16 masculino - Armários e area de descanso</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>vestiario B17 feminino - Chuveiros</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>vestiario B17 feminino - Armários e area de descanso</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>vestiario B18 - parte vestiario fem</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>banheiro B18 feminino - virou DML</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>vestiario B19 masculino - trancado</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>vestiario B19 feminino - trancado</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>36</t>
         </is>
       </c>
     </row>
@@ -466,7 +1063,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -492,42 +1089,19 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2024-12-18</t>
+          <t>2024-12-24</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Maçanetas: TROCA; Divisórias: LIMPEZA</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2024-12-18</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2024-12-18</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Maçanetas: REPARO; Dobradiças: LIMPEZA; Estado Sifão: LIMPEZA</t>
+          <t>Maçanetas: LIMPEZA</t>
         </is>
       </c>
     </row>

</xml_diff>